<commit_message>
Major changes are going to take place from now on
</commit_message>
<xml_diff>
--- a/misc/Stories.xlsx
+++ b/misc/Stories.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\my-react-app\misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F03173E-7F89-47F6-8292-770C40433D75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CC676BE-1DBF-46A8-BAED-1B0CD2B44806}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Remove the header, which contains menu like header, navigation, tasks, and instead, divide them into a separtae components using React JS only.  Eg, heaer component, navigation component, tasks component, etc.</t>
   </si>
@@ -86,6 +86,9 @@
   </si>
   <si>
     <t>Arrange the components in the left, right, left, and then right, so on.</t>
+  </si>
+  <si>
+    <t>Create a roadmap, preferrably in a shape form like tree, leaf, Myshow4all Logo, etc., at the top through which any component can be accessed with a referrenced link to each component</t>
   </si>
 </sst>
 </file>
@@ -429,10 +432,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCDFBBC9-988B-4328-97A4-F82CE7243BC6}">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="25.5" x14ac:dyDescent="1.2"/>
@@ -499,6 +502,11 @@
       <c r="F8" s="2"/>
       <c r="G8" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="76.5" x14ac:dyDescent="1.2">
+      <c r="A9" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>